<commit_message>
Update imports, and clean up float parsing for unrecognized numbers
</commit_message>
<xml_diff>
--- a/tests/testdata/xlsx/Data Type Test.xlsx
+++ b/tests/testdata/xlsx/Data Type Test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3f20bad91a8942d2/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taqi_\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E431694-3921-4B6E-B073-06FB26F18EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40AD360-31D0-4A9C-BACF-8B9FA178D5FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{C249DF93-B9E1-475F-93AA-264E1C9B9BA9}"/>
+    <workbookView xWindow="22330" yWindow="0" windowWidth="16070" windowHeight="14920" xr2:uid="{C249DF93-B9E1-475F-93AA-264E1C9B9BA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,9 +80,6 @@
     <t>$456</t>
   </si>
   <si>
-    <t>foo bar nothing</t>
-  </si>
-  <si>
     <t>2 square feet</t>
   </si>
   <si>
@@ -105,6 +102,9 @@
   </si>
   <si>
     <t>On July 1, 2012</t>
+  </si>
+  <si>
+    <t>foo bar</t>
   </si>
 </sst>
 </file>
@@ -489,7 +489,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -526,13 +526,13 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -543,13 +543,13 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -560,7 +560,7 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -573,16 +573,16 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correctly close sesh, and improve test
</commit_message>
<xml_diff>
--- a/tests/testdata/xlsx/Data Type Test.xlsx
+++ b/tests/testdata/xlsx/Data Type Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taqi_\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40AD360-31D0-4A9C-BACF-8B9FA178D5FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CDCDA91-3AAF-4144-B9BF-C83C7DA10535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22330" yWindow="0" windowWidth="16070" windowHeight="14920" xr2:uid="{C249DF93-B9E1-475F-93AA-264E1C9B9BA9}"/>
+    <workbookView xWindow="22330" yWindow="410" windowWidth="16070" windowHeight="14920" xr2:uid="{C249DF93-B9E1-475F-93AA-264E1C9B9BA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Test Bool</t>
   </si>
@@ -62,9 +62,6 @@
     <t>this is false</t>
   </si>
   <si>
-    <t>this is nothing</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
     <t>measures 20 sqft</t>
   </si>
   <si>
-    <t>wrong value $100</t>
-  </si>
-  <si>
     <t>lorem</t>
   </si>
   <si>
@@ -105,6 +99,18 @@
   </si>
   <si>
     <t>foo bar</t>
+  </si>
+  <si>
+    <t>wrong format $100</t>
+  </si>
+  <si>
+    <t>wrong unit $100</t>
+  </si>
+  <si>
+    <t>different format $100 but save as string</t>
+  </si>
+  <si>
+    <t>blah blah</t>
   </si>
 </sst>
 </file>
@@ -489,7 +495,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -498,7 +504,7 @@
     <col min="2" max="2" width="20.26953125" customWidth="1"/>
     <col min="3" max="3" width="17.26953125" customWidth="1"/>
     <col min="4" max="4" width="22.26953125" customWidth="1"/>
-    <col min="5" max="5" width="24.1796875" customWidth="1"/>
+    <col min="5" max="5" width="30.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -523,16 +529,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -540,49 +546,49 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix data type conversion for values with nested quotes
</commit_message>
<xml_diff>
--- a/tests/testdata/xlsx/Data Type Test.xlsx
+++ b/tests/testdata/xlsx/Data Type Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taqi_\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6205D811-514B-4E2D-B7B6-630C0357D0DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAFDEC7C-4340-4031-BB67-90A9ADE976E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19260" yWindow="3600" windowWidth="16070" windowHeight="14920" xr2:uid="{C249DF93-B9E1-475F-93AA-264E1C9B9BA9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{C249DF93-B9E1-475F-93AA-264E1C9B9BA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t>ipsum</t>
   </si>
   <si>
-    <t>dolor</t>
-  </si>
-  <si>
     <t>July the 1, 1982</t>
   </si>
   <si>
@@ -111,6 +108,9 @@
   </si>
   <si>
     <t>wrong unit $100.5</t>
+  </si>
+  <si>
+    <t>dolor with "quoted" string to test escaping</t>
   </si>
 </sst>
 </file>
@@ -495,7 +495,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -504,7 +504,7 @@
     <col min="2" max="2" width="20.26953125" customWidth="1"/>
     <col min="3" max="3" width="17.26953125" customWidth="1"/>
     <col min="4" max="4" width="22.26953125" customWidth="1"/>
-    <col min="5" max="5" width="30.81640625" customWidth="1"/>
+    <col min="5" max="5" width="41.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -532,10 +532,10 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -549,10 +549,10 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
@@ -560,13 +560,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -579,16 +579,16 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>